<commit_message>
Employee addition code is added successfully.
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>uername</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>2026-10-26</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>bloodGroup</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>tess</t>
+  </si>
+  <si>
+    <t>Testing Data</t>
   </si>
 </sst>
 </file>
@@ -133,11 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +546,7 @@
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -546,8 +562,17 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -562,6 +587,15 @@
       </c>
       <c r="E2" t="s">
         <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for search admin user
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>uername</t>
   </si>
@@ -84,6 +85,18 @@
   </si>
   <si>
     <t>Testing Data</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>Staus</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Enabled</t>
   </si>
 </sst>
 </file>
@@ -536,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,4 +615,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>